<commit_message>
comments made in BOM ZR_V2
</commit_message>
<xml_diff>
--- a/bom/BOM_ZR_V2.xlsx
+++ b/bom/BOM_ZR_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{DEED0C66-80C8-483C-8EF0-F0F9D4B13AD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B249F8EC-3B5B-4833-9A17-CB76DA7508F4}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{DEED0C66-80C8-483C-8EF0-F0F9D4B13AD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F45926CF-6AA6-4556-8D7C-61C01E7B681F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="191">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -603,6 +603,15 @@
       </rPr>
       <t>Thanks to Steven Kleinert for the info.</t>
     </r>
+  </si>
+  <si>
+    <t>Commonly available (same springs as most printers)</t>
+  </si>
+  <si>
+    <t>BK10 and BF10 machined end required.   BK10 and BF10 blocks ARE NOT required.</t>
+  </si>
+  <si>
+    <t>Ball Bearing dont need to be magnetized, Stainless Steal or Chrome Steal preffered.</t>
   </si>
 </sst>
 </file>
@@ -698,7 +707,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -708,6 +717,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -760,7 +775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -832,6 +847,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -976,15 +994,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1007,7 +1025,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="263525"/>
+          <a:off x="3495677" y="5784850"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1020,15 +1038,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>69852</xdr:colOff>
+      <xdr:colOff>212727</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1051,7 +1069,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3365502" y="12404725"/>
+          <a:off x="3498852" y="13500100"/>
           <a:ext cx="975212" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1064,15 +1082,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1095,7 +1113,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="3133725"/>
+          <a:off x="3495677" y="49504600"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1108,15 +1126,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1139,7 +1157,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="4568825"/>
+          <a:off x="3495677" y="17357725"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1152,15 +1170,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1183,7 +1201,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="6003925"/>
+          <a:off x="3495677" y="3213100"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1196,15 +1214,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1227,7 +1245,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="7439025"/>
+          <a:off x="3495677" y="7070725"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1240,15 +1258,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1271,7 +1289,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="8874125"/>
+          <a:off x="3495677" y="59791600"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1284,15 +1302,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1315,7 +1333,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="10309225"/>
+          <a:off x="3495677" y="34074100"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1328,15 +1346,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1359,7 +1377,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="11744325"/>
+          <a:off x="3495677" y="26358850"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1372,15 +1390,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1403,7 +1421,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="13179425"/>
+          <a:off x="3495677" y="31502350"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1416,15 +1434,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1447,7 +1465,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="14614525"/>
+          <a:off x="3495677" y="27644725"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1460,15 +1478,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1491,7 +1509,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="16049625"/>
+          <a:off x="3495677" y="46932850"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1504,15 +1522,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1535,7 +1553,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="17484725"/>
+          <a:off x="3495677" y="48218725"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1548,15 +1566,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1579,7 +1597,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="18919825"/>
+          <a:off x="3495677" y="35359975"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1592,15 +1610,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1623,7 +1641,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="20354925"/>
+          <a:off x="3495677" y="50790475"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1636,15 +1654,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1667,7 +1685,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="21790025"/>
+          <a:off x="3495677" y="32788225"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1680,15 +1698,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1711,7 +1729,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="23225125"/>
+          <a:off x="3495677" y="39217600"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1724,15 +1742,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1755,7 +1773,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="24660225"/>
+          <a:off x="3495677" y="21215350"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1768,15 +1786,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1799,7 +1817,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="26095325"/>
+          <a:off x="3495677" y="45646975"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1812,15 +1830,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1843,7 +1861,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="27530425"/>
+          <a:off x="3495677" y="52076350"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1856,15 +1874,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1887,7 +1905,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="28965525"/>
+          <a:off x="3495677" y="40503475"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1900,15 +1918,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1931,7 +1949,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="30400625"/>
+          <a:off x="3495677" y="53362225"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1944,15 +1962,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1975,7 +1993,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="31835725"/>
+          <a:off x="3495677" y="61077475"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1988,15 +2006,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2019,7 +2037,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="33270825"/>
+          <a:off x="3495677" y="57219850"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2032,15 +2050,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2063,7 +2081,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="34705925"/>
+          <a:off x="3495677" y="18643600"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2076,15 +2094,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2107,7 +2125,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="36141025"/>
+          <a:off x="3495677" y="58505725"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2120,15 +2138,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2151,7 +2169,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="37576125"/>
+          <a:off x="3495677" y="19929475"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2164,15 +2182,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2195,7 +2213,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="39011225"/>
+          <a:off x="3495677" y="37931725"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2208,15 +2226,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2239,7 +2257,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="40446325"/>
+          <a:off x="3495677" y="14785975"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2252,15 +2270,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2283,7 +2301,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="41881425"/>
+          <a:off x="3495677" y="16071850"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2296,15 +2314,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2327,7 +2345,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="43316525"/>
+          <a:off x="3495677" y="55933975"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2340,15 +2358,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2371,7 +2389,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="46186725"/>
+          <a:off x="3495677" y="10928350"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2384,15 +2402,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2415,7 +2433,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="47621825"/>
+          <a:off x="3495677" y="641350"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2428,15 +2446,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2459,7 +2477,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="49056925"/>
+          <a:off x="3495677" y="70078600"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2472,15 +2490,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2503,7 +2521,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="50492025"/>
+          <a:off x="3495677" y="1927225"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2516,15 +2534,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2547,7 +2565,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="51927125"/>
+          <a:off x="3495677" y="41789350"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2560,15 +2578,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2591,7 +2609,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="53362225"/>
+          <a:off x="3495677" y="28930600"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2604,15 +2622,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2635,7 +2653,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="54797325"/>
+          <a:off x="3495677" y="67506850"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2648,15 +2666,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2679,7 +2697,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="56232425"/>
+          <a:off x="3495677" y="54648100"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2692,15 +2710,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2723,7 +2741,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="57667525"/>
+          <a:off x="3495677" y="36645850"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2736,15 +2754,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2767,7 +2785,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="59102625"/>
+          <a:off x="3495677" y="8356600"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2780,15 +2798,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2811,7 +2829,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="60537725"/>
+          <a:off x="3495677" y="12214225"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2824,15 +2842,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2855,7 +2873,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="61972825"/>
+          <a:off x="3495677" y="22501225"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2868,15 +2886,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2899,7 +2917,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="63407925"/>
+          <a:off x="3495677" y="66220975"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2912,15 +2930,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2943,7 +2961,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="64843025"/>
+          <a:off x="3495677" y="68792725"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2956,15 +2974,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2987,7 +3005,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="69148325"/>
+          <a:off x="3495677" y="71364475"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3000,15 +3018,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3031,7 +3049,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="70583425"/>
+          <a:off x="3495677" y="44361100"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3044,15 +3062,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3075,7 +3093,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="72018525"/>
+          <a:off x="3495677" y="43075225"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3088,15 +3106,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3119,7 +3137,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="73453625"/>
+          <a:off x="3495677" y="23787100"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3132,15 +3150,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3163,7 +3181,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="74888725"/>
+          <a:off x="3495677" y="9642475"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3176,15 +3194,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3207,7 +3225,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="76323825"/>
+          <a:off x="3495677" y="25072975"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3220,15 +3238,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3251,7 +3269,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="77758925"/>
+          <a:off x="3495677" y="30216475"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3264,15 +3282,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3295,7 +3313,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="79194025"/>
+          <a:off x="3495677" y="62363350"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3308,15 +3326,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3339,7 +3357,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="80629125"/>
+          <a:off x="3495677" y="4498975"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3352,15 +3370,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3383,7 +3401,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="82064225"/>
+          <a:off x="3495677" y="63649225"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3396,15 +3414,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>66677</xdr:colOff>
+      <xdr:colOff>209552</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1045064</xdr:colOff>
+      <xdr:colOff>1187939</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>1012063</xdr:rowOff>
+      <xdr:rowOff>1135888</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3427,7 +3445,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676277" y="83499325"/>
+          <a:off x="3495677" y="64935100"/>
           <a:ext cx="978387" cy="932688"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3787,9 +3805,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="84.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3797,7 +3815,7 @@
     <col min="1" max="1" width="16.42578125" style="17"/>
     <col min="2" max="2" width="16.42578125" style="19"/>
     <col min="3" max="3" width="16.42578125" style="10"/>
-    <col min="4" max="4" width="16.42578125" style="7"/>
+    <col min="4" max="4" width="20.7109375" style="7" customWidth="1"/>
     <col min="5" max="5" width="40" style="14" customWidth="1"/>
     <col min="6" max="6" width="49" style="23" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
@@ -3847,7 +3865,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>165</v>
       </c>
@@ -3876,7 +3894,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>165</v>
       </c>
@@ -3898,11 +3916,14 @@
       <c r="H3" s="9">
         <v>4</v>
       </c>
+      <c r="I3" s="25" t="s">
+        <v>188</v>
+      </c>
       <c r="L3" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>165</v>
       </c>
@@ -3924,11 +3945,14 @@
       <c r="H4" s="9">
         <v>3</v>
       </c>
+      <c r="I4" s="25" t="s">
+        <v>189</v>
+      </c>
       <c r="L4" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>165</v>
       </c>
@@ -3954,7 +3978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>165</v>
       </c>
@@ -3986,7 +4010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>165</v>
       </c>
@@ -4012,7 +4036,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>165</v>
       </c>
@@ -4038,7 +4062,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>165</v>
       </c>
@@ -4067,7 +4091,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>165</v>
       </c>
@@ -4099,7 +4123,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>165</v>
       </c>
@@ -4125,7 +4149,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>165</v>
       </c>
@@ -4154,7 +4178,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>165</v>
       </c>
@@ -4176,11 +4200,14 @@
       <c r="H13" s="9">
         <v>9</v>
       </c>
+      <c r="I13" s="25" t="s">
+        <v>190</v>
+      </c>
       <c r="L13" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>165</v>
       </c>
@@ -4209,7 +4236,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>165</v>
       </c>
@@ -4238,7 +4265,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>165</v>
       </c>
@@ -4264,7 +4291,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>165</v>
       </c>
@@ -4290,7 +4317,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>165</v>
       </c>
@@ -4316,7 +4343,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>165</v>
       </c>
@@ -4345,7 +4372,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>165</v>
       </c>
@@ -4374,7 +4401,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>165</v>
       </c>
@@ -4403,7 +4430,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>165</v>
       </c>
@@ -4432,7 +4459,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>165</v>
       </c>
@@ -4458,7 +4485,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>165</v>
       </c>
@@ -4484,7 +4511,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>165</v>
       </c>
@@ -4510,7 +4537,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>165</v>
       </c>
@@ -4536,7 +4563,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>165</v>
       </c>
@@ -4562,7 +4589,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>165</v>
       </c>
@@ -4588,7 +4615,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>165</v>
       </c>
@@ -4614,7 +4641,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>165</v>
       </c>
@@ -4640,7 +4667,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>165</v>
       </c>
@@ -4666,7 +4693,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>165</v>
       </c>
@@ -4692,7 +4719,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>165</v>
       </c>
@@ -4718,7 +4745,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>165</v>
       </c>
@@ -4744,7 +4771,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>165</v>
       </c>
@@ -4779,7 +4806,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>165</v>
       </c>
@@ -4814,7 +4841,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>165</v>
       </c>
@@ -4849,7 +4876,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>165</v>
       </c>
@@ -4881,7 +4908,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>165</v>
       </c>
@@ -4913,7 +4940,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>165</v>
       </c>
@@ -4945,7 +4972,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>165</v>
       </c>
@@ -4977,7 +5004,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>165</v>
       </c>
@@ -5009,7 +5036,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>165</v>
       </c>
@@ -5041,7 +5068,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>165</v>
       </c>
@@ -5073,7 +5100,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>165</v>
       </c>
@@ -5105,7 +5132,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>165</v>
       </c>
@@ -5137,7 +5164,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>165</v>
       </c>
@@ -5169,7 +5196,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>165</v>
       </c>
@@ -5204,7 +5231,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>165</v>
       </c>
@@ -5239,7 +5266,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>165</v>
       </c>
@@ -5274,7 +5301,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>165</v>
       </c>
@@ -5309,7 +5336,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>165</v>
       </c>
@@ -5344,7 +5371,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>165</v>
       </c>
@@ -5379,7 +5406,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>165</v>
       </c>
@@ -5411,7 +5438,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
         <v>165</v>
       </c>
@@ -5440,7 +5467,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>165</v>
       </c>
@@ -5475,7 +5502,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>165</v>
       </c>
@@ -5516,7 +5543,7 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
   <drawing r:id="rId4"/>
   <webPublishItems count="1">
-    <webPublishItem id="6083" divId="BOM_ZR_V2_6083" sourceType="sheet" destinationFile="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/BOM_ZR_V2.htm" autoRepublish="1"/>
+    <webPublishItem id="6083" divId="BOM_ZR_V2_6083" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_ZR_V2.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
     <tablePart r:id="rId5"/>

</xml_diff>

<commit_message>
V2 Bom fixed (was refering to V2.5 list)
</commit_message>
<xml_diff>
--- a/bom/BOM_ZR_V2.xlsx
+++ b/bom/BOM_ZR_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{DEED0C66-80C8-483C-8EF0-F0F9D4B13AD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F45926CF-6AA6-4556-8D7C-61C01E7B681F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20760212-F1E0-476D-883B-E0217B8F3859}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -3810,24 +3810,24 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="84.6" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="84.65" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="17"/>
-    <col min="2" max="2" width="16.42578125" style="19"/>
-    <col min="3" max="3" width="16.42578125" style="10"/>
-    <col min="4" max="4" width="20.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" style="17"/>
+    <col min="2" max="2" width="16.453125" style="19"/>
+    <col min="3" max="3" width="16.453125" style="10"/>
+    <col min="4" max="4" width="20.7265625" style="7" customWidth="1"/>
     <col min="5" max="5" width="40" style="14" customWidth="1"/>
     <col min="6" max="6" width="49" style="23" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" style="9"/>
-    <col min="9" max="9" width="56.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="7"/>
-    <col min="11" max="11" width="39.85546875" style="7" customWidth="1"/>
-    <col min="12" max="12" width="33.85546875" style="7" hidden="1" customWidth="1"/>
-    <col min="13" max="16384" width="16.42578125" style="7"/>
+    <col min="7" max="7" width="14.81640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" style="9"/>
+    <col min="9" max="9" width="56.1796875" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" style="7"/>
+    <col min="11" max="11" width="39.81640625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="33.81640625" style="7" hidden="1" customWidth="1"/>
+    <col min="13" max="16384" width="16.453125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>159</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>165</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>165</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>165</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>165</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>165</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>165</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>165</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>165</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>165</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>165</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>165</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>165</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
         <v>165</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
         <v>165</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
         <v>165</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
         <v>165</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
         <v>165</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
         <v>165</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
         <v>165</v>
       </c>
@@ -4401,7 +4401,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
         <v>165</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
         <v>165</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
         <v>165</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
         <v>165</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
         <v>165</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
         <v>165</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
         <v>165</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
         <v>165</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
         <v>165</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
         <v>165</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
         <v>165</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
         <v>165</v>
       </c>
@@ -4719,7 +4719,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
         <v>165</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
         <v>165</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
         <v>165</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
         <v>165</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
         <v>165</v>
       </c>
@@ -4876,7 +4876,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
         <v>165</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
         <v>165</v>
       </c>
@@ -4940,7 +4940,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="17" t="s">
         <v>165</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="17" t="s">
         <v>165</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="17" t="s">
         <v>165</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="17" t="s">
         <v>165</v>
       </c>
@@ -5068,7 +5068,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
         <v>165</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
         <v>165</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="17" t="s">
         <v>165</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
         <v>165</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
         <v>165</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
         <v>165</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="17" t="s">
         <v>165</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="17" t="s">
         <v>165</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="17" t="s">
         <v>165</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="17" t="s">
         <v>165</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="17" t="s">
         <v>165</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="17" t="s">
         <v>165</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="17" t="s">
         <v>165</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>165</v>
       </c>

</xml_diff>